<commit_message>
feat(translation): Add delta script to repo
</commit_message>
<xml_diff>
--- a/utils/localisation_script/hi/Dekho India DELTA Content 21st June Hindi.xlsx
+++ b/utils/localisation_script/hi/Dekho India DELTA Content 21st June Hindi.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/hi/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551DFA39-8E7D-294F-B66E-3556A8FD2420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delta" sheetId="6" r:id="rId1"/>
@@ -328,7 +334,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16">
     <font>
       <sz val="10"/>
@@ -748,111 +754,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A2:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="49.140625" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="14.42578125" style="8"/>
+    <col min="1" max="1" width="16.1640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="37.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="49.1640625" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="A1" s="7"/>
-      <c r="B1" s="13" t="s">
+    <row r="2" spans="1:26" ht="14">
+      <c r="A2" s="7"/>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="7"/>
-    </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="9" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="7"/>
+    </row>
+    <row r="3" spans="1:26" ht="14">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-    </row>
-    <row r="3" spans="1:26" ht="25.5">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -875,18 +849,18 @@
       <c r="Y3" s="10"/>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="28">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -909,13 +883,19 @@
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="14">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
@@ -940,16 +920,10 @@
     <row r="6" spans="1:26">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -971,16 +945,18 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="14">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1003,18 +979,16 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="14">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="6" t="s">
-        <v>16</v>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1037,18 +1011,18 @@
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="43.15" customHeight="1">
+    <row r="9" spans="1:26" ht="14">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>44</v>
+      <c r="F9" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -1071,18 +1045,18 @@
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
     </row>
-    <row r="10" spans="1:26" ht="36" customHeight="1">
+    <row r="10" spans="1:26" ht="43.25" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1105,18 +1079,18 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
     </row>
-    <row r="11" spans="1:26" ht="37.9" customHeight="1">
+    <row r="11" spans="1:26" ht="36" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1139,18 +1113,18 @@
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
     </row>
-    <row r="12" spans="1:26" ht="30.75">
+    <row r="12" spans="1:26" ht="38" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1173,16 +1147,18 @@
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" ht="32">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
+      <c r="D13" s="6" t="s">
+        <v>21</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10" t="s">
-        <v>48</v>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -1205,18 +1181,16 @@
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="14">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>24</v>
+      <c r="C14" s="10"/>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1239,13 +1213,19 @@
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" ht="14">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="C15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1267,19 +1247,13 @@
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
     </row>
-    <row r="16" spans="1:26" ht="46.5">
+    <row r="16" spans="1:26">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1301,16 +1275,18 @@
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" ht="34">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="C17" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1333,13 +1309,17 @@
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" ht="14">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="F18" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1363,19 +1343,11 @@
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="11" t="s">
-        <v>52</v>
-      </c>
+      <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1397,13 +1369,21 @@
       <c r="Y19" s="10"/>
       <c r="Z19" s="10"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="14">
       <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="B20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -1428,18 +1408,10 @@
     <row r="21" spans="1:26">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -1461,18 +1433,20 @@
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="14">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
+      <c r="C22" s="10" t="s">
+        <v>29</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>32</v>
+      <c r="D22" s="6" t="s">
+        <v>30</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10" t="s">
-        <v>54</v>
+      <c r="E22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -1495,13 +1469,19 @@
       <c r="Y22" s="10"/>
       <c r="Z22" s="10"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="14">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
@@ -1523,21 +1503,13 @@
       <c r="Y23" s="10"/>
       <c r="Z23" s="10"/>
     </row>
-    <row r="24" spans="1:26" ht="39" customHeight="1">
+    <row r="24" spans="1:26">
       <c r="A24" s="10"/>
-      <c r="B24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -1559,18 +1531,20 @@
       <c r="Y24" s="10"/>
       <c r="Z24" s="10"/>
     </row>
-    <row r="25" spans="1:26" ht="42">
+    <row r="25" spans="1:26" ht="39" customHeight="1">
       <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="2" t="s">
-        <v>35</v>
+      <c r="B25" s="2" t="s">
+        <v>33</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>36</v>
+      <c r="C25" s="4" t="s">
+        <v>3</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>56</v>
+      <c r="D25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -1593,18 +1567,18 @@
       <c r="Y25" s="10"/>
       <c r="Z25" s="10"/>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" ht="41">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="4" t="s">
-        <v>6</v>
+      <c r="C26" s="4"/>
+      <c r="D26" s="2" t="s">
+        <v>35</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>37</v>
+      <c r="E26" s="2" t="s">
+        <v>36</v>
       </c>
-      <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -1627,13 +1601,19 @@
       <c r="Y26" s="10"/>
       <c r="Z26" s="10"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" ht="14">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
+      <c r="C27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="F27" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
@@ -1655,19 +1635,13 @@
       <c r="Y27" s="10"/>
       <c r="Z27" s="10"/>
     </row>
-    <row r="28" spans="1:26" ht="38.450000000000003" customHeight="1">
+    <row r="28" spans="1:26">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -1689,13 +1663,19 @@
       <c r="Y28" s="10"/>
       <c r="Z28" s="10"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" ht="38.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="C29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="F29" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
@@ -28905,9 +28885,37 @@
       <c r="Y1000" s="10"/>
       <c r="Z1000" s="10"/>
     </row>
+    <row r="1001" spans="1:26">
+      <c r="A1001" s="10"/>
+      <c r="B1001" s="10"/>
+      <c r="C1001" s="10"/>
+      <c r="D1001" s="10"/>
+      <c r="E1001" s="10"/>
+      <c r="F1001" s="10"/>
+      <c r="G1001" s="10"/>
+      <c r="H1001" s="10"/>
+      <c r="I1001" s="10"/>
+      <c r="J1001" s="10"/>
+      <c r="K1001" s="10"/>
+      <c r="L1001" s="10"/>
+      <c r="M1001" s="10"/>
+      <c r="N1001" s="10"/>
+      <c r="O1001" s="10"/>
+      <c r="P1001" s="10"/>
+      <c r="Q1001" s="10"/>
+      <c r="R1001" s="10"/>
+      <c r="S1001" s="10"/>
+      <c r="T1001" s="10"/>
+      <c r="U1001" s="10"/>
+      <c r="V1001" s="10"/>
+      <c r="W1001" s="10"/>
+      <c r="X1001" s="10"/>
+      <c r="Y1001" s="10"/>
+      <c r="Z1001" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>